<commit_message>
feat: add definition import batch and stage support
</commit_message>
<xml_diff>
--- a/Assets/Table/enemyDefinitions.xlsx
+++ b/Assets/Table/enemyDefinitions.xlsx
@@ -49,10 +49,10 @@
     <t xml:space="preserve">Melee</t>
   </si>
   <si>
-    <t xml:space="preserve">(type:Experience;amount:10;probability:1;guaranteed:true)(type:Gold;amount:5;probability:1;guaranteed:true)(type:Health;amount:5;probability:0.1;guaranteed:false)(type:Ability;amount:1;probability:0.05;guaranteed:false)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(type:Ability;amount:1;probability:1;guaranteed:false)</t>
+    <t xml:space="preserve">(type:Experience;amount:10;probability:10000;guaranteed:true)(type:Gold;amount:5;probability:10000;guaranteed:true)(type:Health;amount:5;probability:1000;guaranteed:false)(type:Ability;amount:1;probability:500;guaranteed:false)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(type:Ability;amount:1;probability:10000;guaranteed:false)</t>
   </si>
   <si>
     <t xml:space="preserve">Ranged</t>
@@ -272,7 +272,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -316,16 +316,16 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>50</v>
+        <v>500000</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>5</v>
+        <v>50000</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>1.5</v>
+        <v>15000</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0.5</v>
+        <v>5000</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>9</v>
@@ -339,16 +339,16 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>50</v>
+        <v>500000</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>5</v>
+        <v>50000</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>1.5</v>
+        <v>15000</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>10</v>
@@ -362,16 +362,16 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>50</v>
+        <v>500000</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>5</v>
+        <v>50000</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>1.5</v>
+        <v>15000</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>9</v>

</xml_diff>